<commit_message>
Read me file updated: Data manual
</commit_message>
<xml_diff>
--- a/data/processed/縣市測站選擇.xlsx
+++ b/data/processed/縣市測站選擇.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/windkuo1017/Desktop/NTU_local/fa-25-econ-5166-group-4/data/processed/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92B852FF-4468-324E-B233-5792294488AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DC9DC2B-9AF9-AF4F-981F-C0AB178C6080}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="18380" xr2:uid="{7FD8E6F9-FF03-E443-BD4F-0563544C2147}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="29400" windowHeight="16860" xr2:uid="{7FD8E6F9-FF03-E443-BD4F-0563544C2147}"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="53">
   <si>
     <t>基隆市</t>
   </si>
@@ -166,15 +166,7 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>觀音</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>~2008</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>2009~</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
@@ -271,12 +263,20 @@
       <t>馬祖</t>
     </r>
   </si>
+  <si>
+    <t>2014~</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>2009~2013</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11">
+  <fonts count="12">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -345,6 +345,13 @@
       <sz val="12"/>
       <color rgb="FF0070C0"/>
       <name val="新細明體 (本文)"/>
+      <family val="3"/>
+      <charset val="136"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF0070C0"/>
+      <name val="新細明體"/>
       <family val="3"/>
       <charset val="136"/>
     </font>
@@ -381,9 +388,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
@@ -398,7 +402,7 @@
     <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1">
@@ -406,6 +410,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -742,235 +749,243 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBB2BCBF-5C3D-2B4E-BF22-D4A230AC2AC4}">
-  <dimension ref="A1:D25"/>
+  <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+      <selection activeCell="C26" sqref="A1:C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="16384" width="10.83203125" style="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" s="1" t="s">
+      <c r="A1" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="16">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" s="1" customFormat="1">
+      <c r="A3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="16">
+      <c r="A6" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="C6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="16">
+      <c r="A7" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="C7" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="16">
+      <c r="A8" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="C8" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="16">
+      <c r="A9" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" s="7"/>
+      <c r="D9" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="16">
+      <c r="A10" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" s="7"/>
+    </row>
+    <row r="11" spans="1:4" ht="16">
+      <c r="A11" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="16">
+      <c r="A12" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="16">
+      <c r="A13" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B13" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="16">
+      <c r="A14" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B14" s="10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="16">
+      <c r="A15" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B15" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="16">
+      <c r="A16" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B16" s="10" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="16">
+      <c r="A17" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B17" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="16">
+      <c r="A18" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B18" s="10" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="16">
+      <c r="A19" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B19" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="16">
+      <c r="A20" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="16">
+      <c r="A21" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B21" s="2" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="3" spans="1:4" s="2" customFormat="1">
-      <c r="A3" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="16">
-      <c r="A6" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="B6" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="16">
-      <c r="A7" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="B7" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="16">
-      <c r="A8" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="B8" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="C8" s="8"/>
-      <c r="D8" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="16">
-      <c r="A9" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="B9" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="C9" s="8"/>
-    </row>
-    <row r="10" spans="1:4" ht="16">
-      <c r="A10" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="16">
-      <c r="A11" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="B11" s="11" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="16">
-      <c r="A12" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="16">
-      <c r="A13" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B13" s="11" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="16">
-      <c r="A14" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="16">
-      <c r="A15" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="B15" s="11" t="s">
+    <row r="22" spans="1:2" ht="16">
+      <c r="A22" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B22" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="16">
-      <c r="A16" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" ht="16">
-      <c r="A17" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="B17" s="11" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" ht="16">
-      <c r="A18" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="B18" s="1" t="s">
+    <row r="23" spans="1:2" ht="16">
+      <c r="A23" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" t="s">
+        <v>19</v>
+      </c>
+      <c r="B24" s="9" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="16">
-      <c r="A19" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" ht="16">
-      <c r="A20" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="B20" s="3" t="s">
+    <row r="25" spans="1:2" ht="16">
+      <c r="A25" t="s">
+        <v>20</v>
+      </c>
+      <c r="B25" s="2" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="16">
-      <c r="A21" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" ht="16">
-      <c r="A22" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="B22" s="3" t="s">
+    <row r="26" spans="1:2" ht="16">
+      <c r="A26" t="s">
+        <v>25</v>
+      </c>
+      <c r="B26" s="2" t="s">
         <v>50</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2">
-      <c r="A23" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B23" s="10" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" ht="16">
-      <c r="A24" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B24" s="3" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" ht="16">
-      <c r="A25" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>